<commit_message>
refactoring to retrieve all rows typed for futher iteration; Created wrappers;
</commit_message>
<xml_diff>
--- a/src/main/resources/all-columns-fulfilled.xlsx
+++ b/src/main/resources/all-columns-fulfilled.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Column A</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Column H</t>
+  </si>
+  <si>
+    <t>Column I</t>
   </si>
   <si>
     <t>Acá ferro</t>
@@ -123,7 +126,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +179,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCC9966"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -224,7 +233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -266,6 +275,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,12 +363,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65536"/>
+  <dimension ref="A1:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -368,7 +381,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5344129554656"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4372469635628"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="52.8461538461538"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.40485829959514"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.1295546558704"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.1376518218623"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.5222672064777"/>
@@ -413,6 +426,9 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
@@ -425,7 +441,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="7" t="n">
         <v>0</v>
@@ -434,11 +450,12 @@
         <v>0</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H2" s="10" t="n">
         <v>42494.4237268519</v>
       </c>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
@@ -450,8 +467,8 @@
       <c r="C3" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>10</v>
+      <c r="D3" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="E3" s="7" t="n">
         <v>100</v>
@@ -460,11 +477,12 @@
         <v>1</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" s="10" t="n">
         <v>42495.466099537</v>
       </c>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
@@ -476,8 +494,8 @@
       <c r="C4" s="5" t="n">
         <v>1000</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>12</v>
+      <c r="D4" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="E4" s="7" t="n">
         <v>1000</v>
@@ -486,11 +504,12 @@
         <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="10" t="n">
         <v>42496.5084722222</v>
       </c>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -502,8 +521,8 @@
       <c r="C5" s="5" t="n">
         <v>10000</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>14</v>
+      <c r="D5" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="E5" s="7" t="n">
         <v>10000</v>
@@ -512,11 +531,12 @@
         <v>100</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="10" t="n">
         <v>42497.5508449074</v>
       </c>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
@@ -528,8 +548,8 @@
       <c r="C6" s="5" t="n">
         <v>100000</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>16</v>
+      <c r="D6" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="E6" s="7" t="n">
         <v>100000</v>
@@ -538,11 +558,12 @@
         <v>1000</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="10" t="n">
         <v>42498.5932175926</v>
       </c>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
@@ -554,8 +575,8 @@
       <c r="C7" s="5" t="n">
         <v>1000000</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>18</v>
+      <c r="D7" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="E7" s="7" t="n">
         <v>1000000</v>
@@ -564,11 +585,12 @@
         <v>10000</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H7" s="10" t="n">
         <v>42499.6355902778</v>
       </c>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -580,8 +602,8 @@
       <c r="C8" s="5" t="n">
         <v>10000000</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>20</v>
+      <c r="D8" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="E8" s="7" t="n">
         <v>100000000</v>
@@ -590,11 +612,12 @@
         <v>100000</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" s="10" t="n">
         <v>42500.677962963</v>
       </c>
+      <c r="I8" s="11"/>
     </row>
     <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>